<commit_message>
Updated code for AN4_Fili_Updated
</commit_message>
<xml_diff>
--- a/src/test/java/testData/TestSuite1.xlsx
+++ b/src/test/java/testData/TestSuite1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arorag\eclipse-workspace\AN4_FILI_UPDATED\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA3DF7E-9653-413E-BEE9-7CC60605BDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16551CD5-4E10-4FBA-A7C4-8FEED9F9D360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="763" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8585" uniqueCount="1648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8588" uniqueCount="1624">
   <si>
     <t>TCID</t>
   </si>
@@ -4712,15 +4712,9 @@
     <t>Payment2_Suitability_Annuitypurchaseamount</t>
   </si>
   <si>
-    <t>payment2suitabilityquestions.allcarriershavepremiumthresholdsthatmayrequirelargecasepre-approval.</t>
-  </si>
-  <si>
     <t>Payment2 Suitability Questions - Name of the company where the Brokerage Account is held</t>
   </si>
   <si>
-    <t>Payment2 Suitability Questions - All carriers have premium thresholds that may require large case pre-approval.</t>
-  </si>
-  <si>
     <t>Click Next Button in Payment2 Suitability screen</t>
   </si>
   <si>
@@ -4742,9 +4736,6 @@
     <t>TSQ - What is the total number of the Owner's and Joint Owner's dependents?</t>
   </si>
   <si>
-    <t>transactionsuitability.whatisthetotalnumberof theOwner'sandJointOwner'sdependents?</t>
-  </si>
-  <si>
     <t>TSQ_Whatisthetotalnumber</t>
   </si>
   <si>
@@ -4754,57 +4745,18 @@
     <t>TSQ -Is the Owner Retired?</t>
   </si>
   <si>
-    <t>transactionsuitability.istheownerretired?</t>
-  </si>
-  <si>
-    <t>TSQ - If employed, occupation (otherwise please enter "Not Employed").</t>
-  </si>
-  <si>
-    <t>transactionsuitability.Is the Owner Married?</t>
-  </si>
-  <si>
-    <t>transactionsuitability.Ifemployed,occupation(otherwisepleaseenter"NotEmployed").</t>
-  </si>
-  <si>
-    <t>TSQ_Ifemployed,occupation(otherwisepleaseenter"NotEmployed").</t>
-  </si>
-  <si>
     <t>TSQ - What is your risk tolerance/allocation strategy for this investment?</t>
   </si>
   <si>
-    <t>transactionsuitability.whatisyourrisktolerance/allocationstrategyforthisinvestment?</t>
-  </si>
-  <si>
     <t>TSQ -Do you have an emergency fund to satisfy any emergencies and major expenses</t>
   </si>
   <si>
-    <t>transactionsuitability.doyou haveanemergencyfundtosatisfyanyemergenciesandmajorexpenses</t>
-  </si>
-  <si>
     <t>TSQ - What is your annual income (from all sources)?</t>
   </si>
   <si>
-    <t>transactionsuitability.whatisyourannualincome(from all sources)?</t>
-  </si>
-  <si>
-    <t>transactionsuitability.whatisyourinvestmentobjectiveforthisinvestment?</t>
-  </si>
-  <si>
-    <t>transactionsuitability.areyoupurchasingthiscontractfor theGuaranteedLifetimeWithdrawal Benefit?</t>
-  </si>
-  <si>
     <t>TSQ - What is your time horizon for this investment (How long do you plan to keep this annuity)?</t>
   </si>
   <si>
-    <t>transactionsuitability.whatisyourtimehorizonforthisinvestment(Howlongdoyouplantokeepthisannuity)?</t>
-  </si>
-  <si>
-    <t>transactionsuitability.whatisyourfederaltaxbracket?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transactionsuitability.whatareyourmonthlynondiscretionaryexpenses </t>
-  </si>
-  <si>
     <t xml:space="preserve">TSQ - What are your monthly nondiscretionary expenses </t>
   </si>
   <si>
@@ -4814,33 +4766,18 @@
     <t>TSQ -Have you received a current prospectus and privacy notice and reviewed and understand all the material features associated with this variable deferred annuity?</t>
   </si>
   <si>
-    <t>transactionsuitability.haveyoureceivedacurrentprospectusandprivacynotice</t>
-  </si>
-  <si>
     <t>TSQ -Will you be purchasing this annuity with funds derived from or associated with a reverse mortgage?</t>
   </si>
   <si>
-    <t>transactionsuitability.willyoubepurchasingthisannuitywithfunds</t>
-  </si>
-  <si>
     <t>TSQ -Do you intend to apply for means-tested government benefits</t>
   </si>
   <si>
-    <t>transactionsuitability.doyouintendtoapplyformeans-testedgovernmentbenefits</t>
-  </si>
-  <si>
     <t>TSQ -I/We have sufficient liquid funds to satisfy any emergencies and major expenses</t>
   </si>
   <si>
-    <t>transactionsuitability.I/Wehavesufficientliquidfundstosatisfyanyemergenciesandmajorexpenses</t>
-  </si>
-  <si>
     <t xml:space="preserve">TSQ -I/We understand that the only value accessible in the annuity is the contract value. </t>
   </si>
   <si>
-    <t xml:space="preserve">transactionsuitability.I/Weunderstandthattheonlyvalueaccessibleintheannuityisthecontractvalue. </t>
-  </si>
-  <si>
     <t xml:space="preserve">TSQ -  I/We understand that this annuity does not provide a guaranteed rate of return </t>
   </si>
   <si>
@@ -4862,33 +4799,6 @@
     <t>TSQ - Qualified contracts only: I understand that if withdrawals from this annuity</t>
   </si>
   <si>
-    <t>transactionsuitability. I/WeunderstandthatthepolicychargesaGLWBriderfee</t>
-  </si>
-  <si>
-    <t>transactionsuitability.Qualifiedcontractsonly:Iunderstandthatifwithdrawalsfromthisannuity</t>
-  </si>
-  <si>
-    <t>transactionsuitability.I/WeunderstandthattheannuitychargesaMortalityandExpenseFee</t>
-  </si>
-  <si>
-    <t>transactionsuitability.I/WeunderstandthatEarlyWithdrawals</t>
-  </si>
-  <si>
-    <t>transactionsuitability.I/Weunderstand that prior to initiating GLWB withdrawals</t>
-  </si>
-  <si>
-    <t>transactionsuitability.I/Weunderstandthatthereisoneinvestmentoption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transactionsuitability.I/Weunderstandthatthisannuitydoesnot provideaguaranteedrateofreturn </t>
-  </si>
-  <si>
-    <t>transactionsuitability.Immediate/deferredincomeannuities</t>
-  </si>
-  <si>
-    <t>transactionsuitability.Systematicwithdrawalplanfromamutualfundportfolio</t>
-  </si>
-  <si>
     <t>Beneficiary1_RelationtoAnnuitant</t>
   </si>
   <si>
@@ -4980,6 +4890,24 @@
   </si>
   <si>
     <t>Payment2_Suitability_estimatedsurrenderchargeamount</t>
+  </si>
+  <si>
+    <t>Click Next Button in Payment 2 additional information screen</t>
+  </si>
+  <si>
+    <t>transactionsuitability.We_understand_that_prior_to_initiating_GLWB_withdrawals</t>
+  </si>
+  <si>
+    <t>transactionsuitability.We_understand_that_Early_Withdrawals</t>
+  </si>
+  <si>
+    <t>transactionsuitability.We_understand_that_the_annuity_charges_a_Mortality_and_Expense_Fee</t>
+  </si>
+  <si>
+    <t>transactionsuitability.We_understand_that_the_policy_charges_a_GLWB_rider_fee</t>
+  </si>
+  <si>
+    <t>transactionsuitability.I_understand_that_if_withdrawals_from_this_annuity</t>
   </si>
 </sst>
 </file>
@@ -5069,7 +4997,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5109,6 +5037,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5152,7 +5086,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5202,6 +5136,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -26959,10 +26898,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5830309E-7394-4D4A-96E5-506F2D1AA871}">
-  <dimension ref="A1:F164"/>
+  <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28098,7 +28037,7 @@
         <v>66</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>1625</v>
+        <v>1595</v>
       </c>
       <c r="E63" s="21" t="s">
         <v>4</v>
@@ -28201,7 +28140,7 @@
         <v>66</v>
       </c>
       <c r="D69" s="32" t="s">
-        <v>1624</v>
+        <v>1594</v>
       </c>
       <c r="E69" s="21" t="s">
         <v>4</v>
@@ -28259,7 +28198,7 @@
         <v>66</v>
       </c>
       <c r="D72" s="32" t="s">
-        <v>1623</v>
+        <v>1593</v>
       </c>
       <c r="E72" s="21" t="s">
         <v>4</v>
@@ -28277,7 +28216,7 @@
         <v>16</v>
       </c>
       <c r="D73" s="32" t="s">
-        <v>1622</v>
+        <v>1592</v>
       </c>
       <c r="E73" s="21" t="s">
         <v>4</v>
@@ -28291,7 +28230,7 @@
         <v>273</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>1619</v>
+        <v>1589</v>
       </c>
       <c r="C74" s="21" t="s">
         <v>70</v>
@@ -28303,7 +28242,7 @@
         <v>4</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>1617</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -28351,7 +28290,7 @@
         <v>66</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>1624</v>
+        <v>1594</v>
       </c>
       <c r="E77" s="21" t="s">
         <v>4</v>
@@ -28375,7 +28314,7 @@
         <v>4</v>
       </c>
       <c r="F78" s="21" t="s">
-        <v>1621</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -28409,7 +28348,7 @@
         <v>66</v>
       </c>
       <c r="D80" s="32" t="s">
-        <v>1623</v>
+        <v>1593</v>
       </c>
       <c r="E80" s="21" t="s">
         <v>4</v>
@@ -28427,7 +28366,7 @@
         <v>16</v>
       </c>
       <c r="D81" s="32" t="s">
-        <v>1622</v>
+        <v>1592</v>
       </c>
       <c r="E81" s="21" t="s">
         <v>4</v>
@@ -28441,7 +28380,7 @@
         <v>60</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>1620</v>
+        <v>1590</v>
       </c>
       <c r="C82" s="21" t="s">
         <v>247</v>
@@ -28473,7 +28412,7 @@
         <v>273</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>1619</v>
+        <v>1589</v>
       </c>
       <c r="C84" s="21" t="s">
         <v>70</v>
@@ -28485,7 +28424,7 @@
         <v>4</v>
       </c>
       <c r="F84" s="21" t="s">
-        <v>1618</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -28691,7 +28630,7 @@
         <v>254</v>
       </c>
       <c r="B96" t="s">
-        <v>1626</v>
+        <v>1596</v>
       </c>
       <c r="C96" s="21" t="s">
         <v>16</v>
@@ -28703,7 +28642,7 @@
         <v>4</v>
       </c>
       <c r="F96" s="31" t="s">
-        <v>1627</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -28711,7 +28650,7 @@
         <v>254</v>
       </c>
       <c r="B97" t="s">
-        <v>1626</v>
+        <v>1596</v>
       </c>
       <c r="C97" s="21" t="s">
         <v>16</v>
@@ -28723,7 +28662,7 @@
         <v>4</v>
       </c>
       <c r="F97" s="31" t="s">
-        <v>1628</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -28731,7 +28670,7 @@
         <v>254</v>
       </c>
       <c r="B98" t="s">
-        <v>1626</v>
+        <v>1596</v>
       </c>
       <c r="C98" s="21" t="s">
         <v>70</v>
@@ -28743,7 +28682,7 @@
         <v>4</v>
       </c>
       <c r="F98" s="31" t="s">
-        <v>1629</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -28751,7 +28690,7 @@
         <v>254</v>
       </c>
       <c r="B99" t="s">
-        <v>1626</v>
+        <v>1596</v>
       </c>
       <c r="C99" s="21" t="s">
         <v>16</v>
@@ -28763,7 +28702,7 @@
         <v>4</v>
       </c>
       <c r="F99" s="31" t="s">
-        <v>1630</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -28777,7 +28716,7 @@
         <v>16</v>
       </c>
       <c r="D100" s="32" t="s">
-        <v>1631</v>
+        <v>1601</v>
       </c>
       <c r="E100" s="31" t="s">
         <v>4</v>
@@ -29057,19 +28996,19 @@
         <v>684</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="C116" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D116" s="32" t="s">
-        <v>1632</v>
+        <v>1602</v>
       </c>
       <c r="E116" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>1636</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -29077,7 +29016,7 @@
         <v>684</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>1634</v>
+        <v>1604</v>
       </c>
       <c r="C117" s="14" t="s">
         <v>16</v>
@@ -29089,7 +29028,7 @@
         <v>4</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>1633</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -29097,7 +29036,7 @@
         <v>684</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>1635</v>
+        <v>1605</v>
       </c>
       <c r="C118" s="14" t="s">
         <v>16</v>
@@ -29117,7 +29056,7 @@
         <v>684</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>1637</v>
+        <v>1607</v>
       </c>
       <c r="C119" s="14" t="s">
         <v>66</v>
@@ -29135,7 +29074,7 @@
         <v>254</v>
       </c>
       <c r="B120" t="s">
-        <v>1642</v>
+        <v>1612</v>
       </c>
       <c r="C120" s="21" t="s">
         <v>16</v>
@@ -29147,7 +29086,7 @@
         <v>4</v>
       </c>
       <c r="F120" s="31" t="s">
-        <v>1638</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -29155,7 +29094,7 @@
         <v>254</v>
       </c>
       <c r="B121" t="s">
-        <v>1642</v>
+        <v>1612</v>
       </c>
       <c r="C121" s="21" t="s">
         <v>16</v>
@@ -29167,7 +29106,7 @@
         <v>4</v>
       </c>
       <c r="F121" s="31" t="s">
-        <v>1639</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -29175,7 +29114,7 @@
         <v>254</v>
       </c>
       <c r="B122" t="s">
-        <v>1626</v>
+        <v>1596</v>
       </c>
       <c r="C122" s="21" t="s">
         <v>70</v>
@@ -29187,7 +29126,7 @@
         <v>4</v>
       </c>
       <c r="F122" s="31" t="s">
-        <v>1640</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -29195,7 +29134,7 @@
         <v>254</v>
       </c>
       <c r="B123" t="s">
-        <v>1642</v>
+        <v>1612</v>
       </c>
       <c r="C123" s="21" t="s">
         <v>16</v>
@@ -29207,7 +29146,7 @@
         <v>4</v>
       </c>
       <c r="F123" s="31" t="s">
-        <v>1641</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -29215,19 +29154,19 @@
         <v>254</v>
       </c>
       <c r="B124" t="s">
-        <v>1643</v>
+        <v>1613</v>
       </c>
       <c r="C124" s="21" t="s">
         <v>16</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>1631</v>
+        <v>1601</v>
       </c>
       <c r="E124" s="31" t="s">
         <v>4</v>
       </c>
       <c r="F124" s="31" t="s">
-        <v>1644</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -29235,7 +29174,7 @@
         <v>254</v>
       </c>
       <c r="B125" t="s">
-        <v>1645</v>
+        <v>1615</v>
       </c>
       <c r="C125" t="s">
         <v>66</v>
@@ -29253,7 +29192,7 @@
         <v>254</v>
       </c>
       <c r="B126" t="s">
-        <v>1646</v>
+        <v>1616</v>
       </c>
       <c r="C126" s="21" t="s">
         <v>16</v>
@@ -29265,40 +29204,38 @@
         <v>4</v>
       </c>
       <c r="F126" s="31" t="s">
-        <v>1647</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="14" t="s">
-        <v>684</v>
-      </c>
-      <c r="B127" s="14" t="s">
-        <v>1560</v>
-      </c>
-      <c r="C127" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>1558</v>
-      </c>
-      <c r="E127" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F127" s="14"/>
+      <c r="A127" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="B127" s="21" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D127" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E127" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F127" s="21"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="21" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B128" s="21" t="s">
-        <v>1561</v>
+        <v>264</v>
       </c>
       <c r="C128" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D128" s="21" t="s">
-        <v>58</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D128" s="21"/>
       <c r="E128" s="21" t="s">
         <v>4</v>
       </c>
@@ -29306,26 +29243,28 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="B129" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="C129" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D129" s="21"/>
-      <c r="E129" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F129" s="21"/>
+        <v>254</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C129" t="s">
+        <v>66</v>
+      </c>
+      <c r="D129" s="31" t="s">
+        <v>459</v>
+      </c>
+      <c r="E129" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F129" s="31"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="21" t="s">
         <v>246</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="C130" s="21" t="s">
         <v>25</v>
@@ -29355,165 +29294,161 @@
       <c r="F131" s="21"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="14" t="s">
+      <c r="A132" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="B132" s="21" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C132" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D132" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E132" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F132" s="21"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="B133" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="C133" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D133" s="21"/>
+      <c r="E133" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F133" s="21"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="14" t="s">
         <v>692</v>
       </c>
-      <c r="B132" s="14" t="s">
+      <c r="B134" s="14" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C134" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D134" s="14" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E134" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F134" s="14" t="s">
         <v>1563</v>
       </c>
-      <c r="C132" s="14" t="s">
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="14" t="s">
+        <v>692</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C135" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D132" s="14" t="s">
+      <c r="D135" s="14" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E135" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F135" s="14"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="B136" s="21" t="s">
         <v>1564</v>
       </c>
-      <c r="E132" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F132" s="14" t="s">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="14" t="s">
-        <v>692</v>
-      </c>
-      <c r="B133" s="14" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C133" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D133" s="14" t="s">
-        <v>1190</v>
-      </c>
-      <c r="E133" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F133" s="14"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="B134" s="21" t="s">
-        <v>1566</v>
-      </c>
-      <c r="C134" s="21" t="s">
+      <c r="C136" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D134" s="21" t="s">
+      <c r="D136" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E134" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F134" s="21"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="21" t="s">
+      <c r="E136" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F136" s="21"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="B135" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="C135" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D135" s="21"/>
-      <c r="E135" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F135" s="21"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="14" t="s">
-        <v>695</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>1567</v>
-      </c>
-      <c r="C136" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D136" s="14" t="s">
-        <v>1568</v>
-      </c>
-      <c r="E136" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F136" s="14" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="14" t="s">
-        <v>695</v>
-      </c>
-      <c r="B137" s="14" t="s">
-        <v>1570</v>
-      </c>
-      <c r="C137" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D137" s="14" t="s">
-        <v>1574</v>
-      </c>
-      <c r="E137" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F137" s="14"/>
+      <c r="B137" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="C137" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D137" s="21"/>
+      <c r="E137" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F137" s="21"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
         <v>695</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>1571</v>
+        <v>1565</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D138" s="14" t="s">
-        <v>1572</v>
+        <v>16</v>
+      </c>
+      <c r="D138" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="E138" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F138" s="14"/>
+      <c r="F138" s="14" t="s">
+        <v>1566</v>
+      </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
         <v>695</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>1573</v>
+        <v>1567</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D139" s="14" t="s">
-        <v>1575</v>
+        <v>66</v>
+      </c>
+      <c r="D139" s="32" t="s">
+        <v>461</v>
       </c>
       <c r="E139" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F139" s="14" t="s">
-        <v>1576</v>
-      </c>
+      <c r="F139" s="14"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
         <v>695</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>1577</v>
+        <v>1568</v>
       </c>
       <c r="C140" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D140" s="14" t="s">
-        <v>1578</v>
+      <c r="D140" s="32" t="s">
+        <v>462</v>
       </c>
       <c r="E140" s="14" t="s">
         <v>4</v>
@@ -29525,13 +29460,13 @@
         <v>695</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>1579</v>
+        <v>1569</v>
       </c>
       <c r="C141" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D141" s="14" t="s">
-        <v>1580</v>
+      <c r="D141" s="32" t="s">
+        <v>859</v>
       </c>
       <c r="E141" s="14" t="s">
         <v>4</v>
@@ -29543,13 +29478,13 @@
         <v>695</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>1577</v>
+        <v>1570</v>
       </c>
       <c r="C142" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D142" s="14" t="s">
-        <v>1578</v>
+      <c r="D142" s="32" t="s">
+        <v>464</v>
       </c>
       <c r="E142" s="14" t="s">
         <v>4</v>
@@ -29561,13 +29496,13 @@
         <v>695</v>
       </c>
       <c r="B143" s="14" t="s">
-        <v>1581</v>
+        <v>1571</v>
       </c>
       <c r="C143" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D143" s="14" t="s">
-        <v>1582</v>
+      <c r="D143" s="32" t="s">
+        <v>466</v>
       </c>
       <c r="E143" s="14" t="s">
         <v>4</v>
@@ -29584,8 +29519,8 @@
       <c r="C144" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D144" s="14" t="s">
-        <v>1583</v>
+      <c r="D144" s="32" t="s">
+        <v>1461</v>
       </c>
       <c r="E144" s="14" t="s">
         <v>4</v>
@@ -29602,8 +29537,8 @@
       <c r="C145" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D145" s="14" t="s">
-        <v>1584</v>
+      <c r="D145" s="32" t="s">
+        <v>1463</v>
       </c>
       <c r="E145" s="14" t="s">
         <v>4</v>
@@ -29615,13 +29550,13 @@
         <v>695</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>1585</v>
+        <v>1572</v>
       </c>
       <c r="C146" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D146" s="14" t="s">
-        <v>1586</v>
+      <c r="D146" s="32" t="s">
+        <v>1465</v>
       </c>
       <c r="E146" s="14" t="s">
         <v>4</v>
@@ -29638,8 +29573,8 @@
       <c r="C147" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D147" s="14" t="s">
-        <v>1587</v>
+      <c r="D147" s="32" t="s">
+        <v>468</v>
       </c>
       <c r="E147" s="14" t="s">
         <v>4</v>
@@ -29656,7 +29591,7 @@
       <c r="C148" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D148" s="14" t="s">
+      <c r="D148" s="32" t="s">
         <v>469</v>
       </c>
       <c r="E148" s="14" t="s">
@@ -29669,13 +29604,13 @@
         <v>695</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>1589</v>
+        <v>1573</v>
       </c>
       <c r="C149" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D149" s="14" t="s">
-        <v>1588</v>
+      <c r="D149" s="32" t="s">
+        <v>471</v>
       </c>
       <c r="E149" s="14" t="s">
         <v>4</v>
@@ -29687,12 +29622,12 @@
         <v>695</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>1590</v>
+        <v>1574</v>
       </c>
       <c r="C150" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D150" s="14" t="s">
+      <c r="D150" s="32" t="s">
         <v>472</v>
       </c>
       <c r="E150" s="14" t="s">
@@ -29705,13 +29640,13 @@
         <v>695</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>1591</v>
+        <v>1575</v>
       </c>
       <c r="C151" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D151" s="14" t="s">
-        <v>1592</v>
+      <c r="D151" s="32" t="s">
+        <v>1491</v>
       </c>
       <c r="E151" s="14" t="s">
         <v>4</v>
@@ -29723,13 +29658,13 @@
         <v>695</v>
       </c>
       <c r="B152" s="14" t="s">
-        <v>1593</v>
+        <v>1576</v>
       </c>
       <c r="C152" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D152" s="14" t="s">
-        <v>1594</v>
+      <c r="D152" s="32" t="s">
+        <v>473</v>
       </c>
       <c r="E152" s="14" t="s">
         <v>4</v>
@@ -29741,13 +29676,13 @@
         <v>695</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>1595</v>
+        <v>1577</v>
       </c>
       <c r="C153" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D153" s="14" t="s">
-        <v>1596</v>
+      <c r="D153" s="32" t="s">
+        <v>474</v>
       </c>
       <c r="E153" s="14" t="s">
         <v>4</v>
@@ -29759,13 +29694,13 @@
         <v>695</v>
       </c>
       <c r="B154" s="14" t="s">
-        <v>1597</v>
+        <v>1578</v>
       </c>
       <c r="C154" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D154" s="14" t="s">
-        <v>1598</v>
+      <c r="D154" s="32" t="s">
+        <v>880</v>
       </c>
       <c r="E154" s="14" t="s">
         <v>4</v>
@@ -29777,13 +29712,13 @@
         <v>695</v>
       </c>
       <c r="B155" s="14" t="s">
-        <v>1599</v>
+        <v>1579</v>
       </c>
       <c r="C155" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D155" s="14" t="s">
-        <v>1600</v>
+      <c r="D155" s="32" t="s">
+        <v>880</v>
       </c>
       <c r="E155" s="14" t="s">
         <v>4</v>
@@ -29795,49 +29730,49 @@
         <v>695</v>
       </c>
       <c r="B156" s="14" t="s">
-        <v>1601</v>
+        <v>1580</v>
       </c>
       <c r="C156" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D156" s="14" t="s">
-        <v>1614</v>
+      <c r="D156" s="32" t="s">
+        <v>1476</v>
       </c>
       <c r="E156" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F156" s="14"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" s="14" t="s">
+    <row r="157" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="33" t="s">
         <v>695</v>
       </c>
-      <c r="B157" s="14" t="s">
-        <v>1602</v>
-      </c>
-      <c r="C157" s="14" t="s">
+      <c r="B157" s="33" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C157" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D157" s="14" t="s">
-        <v>1613</v>
-      </c>
-      <c r="E157" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F157" s="14"/>
+      <c r="D157" s="34" t="s">
+        <v>1477</v>
+      </c>
+      <c r="E157" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F157" s="33"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
         <v>695</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>1603</v>
+        <v>1582</v>
       </c>
       <c r="C158" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D158" s="14" t="s">
-        <v>1612</v>
+      <c r="D158" s="32" t="s">
+        <v>1619</v>
       </c>
       <c r="E158" s="14" t="s">
         <v>4</v>
@@ -29849,13 +29784,13 @@
         <v>695</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>1604</v>
+        <v>1583</v>
       </c>
       <c r="C159" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D159" s="14" t="s">
-        <v>1611</v>
+      <c r="D159" s="32" t="s">
+        <v>1620</v>
       </c>
       <c r="E159" s="14" t="s">
         <v>4</v>
@@ -29867,13 +29802,13 @@
         <v>695</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>1605</v>
+        <v>1584</v>
       </c>
       <c r="C160" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D160" s="14" t="s">
-        <v>1610</v>
+      <c r="D160" s="32" t="s">
+        <v>1621</v>
       </c>
       <c r="E160" s="14" t="s">
         <v>4</v>
@@ -29885,13 +29820,13 @@
         <v>695</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>1606</v>
+        <v>1585</v>
       </c>
       <c r="C161" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D161" s="14" t="s">
-        <v>1608</v>
+      <c r="D161" s="32" t="s">
+        <v>1622</v>
       </c>
       <c r="E161" s="14" t="s">
         <v>4</v>
@@ -29903,13 +29838,13 @@
         <v>695</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>1607</v>
+        <v>1586</v>
       </c>
       <c r="C162" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D162" s="14" t="s">
-        <v>1609</v>
+      <c r="D162" s="32" t="s">
+        <v>1623</v>
       </c>
       <c r="E162" s="14" t="s">
         <v>4</v>
@@ -29926,8 +29861,8 @@
       <c r="C163" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D163" s="14" t="s">
-        <v>1615</v>
+      <c r="D163" s="32" t="s">
+        <v>1482</v>
       </c>
       <c r="E163" s="14" t="s">
         <v>4</v>
@@ -29944,13 +29879,31 @@
       <c r="C164" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D164" s="14" t="s">
-        <v>1616</v>
+      <c r="D164" s="32" t="s">
+        <v>1488</v>
       </c>
       <c r="E164" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F164" s="14"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="14" t="s">
+        <v>695</v>
+      </c>
+      <c r="B165" s="14" t="s">
+        <v>750</v>
+      </c>
+      <c r="C165" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D165" s="32" t="s">
+        <v>1489</v>
+      </c>
+      <c r="E165" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F165" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>